<commit_message>
Adding Hibernate configuration & Validate User with Login
1) Added Hibernate external jar files.

2) Added hibernate configuration in the "MySociety-SpringConfig.xml"
file under the "config" folder.

4)  Added the database.properties file under "src/resources" folder.

3) Added UserDAO and LoginService interfaces.

4) Implemented the UserDAO with class UserDAOImpl and LoginService with
LoginServiceImpl class.

5) Implemented basic CRUD operations in UserDAOImpl class and
ValidateUser operation in LoginServiceImpl class.

6) Added the ValidateLogin in the LoginController class to consume the
Login service to validate the user and open home page if successful and
redirect to LoginError page in case if validation fails.
</commit_message>
<xml_diff>
--- a/Docs/Technical/DBDesign/Login_Registration.xlsx
+++ b/Docs/Technical/DBDesign/Login_Registration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
   <si>
     <t>User</t>
   </si>
@@ -202,13 +202,223 @@
   </si>
   <si>
     <t>mbhatnagar</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>UserId (FK - User Table)</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Wing</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PrimaryEmail</t>
+  </si>
+  <si>
+    <t>PrimaryContact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouneel </t>
+  </si>
+  <si>
+    <t>Mehta</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>mouneel@yahoo.com</t>
+  </si>
+  <si>
+    <t>AlternativeContact1</t>
+  </si>
+  <si>
+    <t>AlternativeContact2</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Occupancy (Self/Rented)</t>
+  </si>
+  <si>
+    <t>FlatId</t>
+  </si>
+  <si>
+    <t>C502</t>
+  </si>
+  <si>
+    <t>FlatMaster</t>
+  </si>
+  <si>
+    <t>FlatNo</t>
+  </si>
+  <si>
+    <t>Flat Area (Sq. Ft.)</t>
+  </si>
+  <si>
+    <t>ParkingNos</t>
+  </si>
+  <si>
+    <t>7, 8</t>
+  </si>
+  <si>
+    <t>FlatTenant</t>
+  </si>
+  <si>
+    <t>FlatTenantId</t>
+  </si>
+  <si>
+    <t>OwnerDetails</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>ContactNo</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>PermanentAddress</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>OfficeAddress</t>
+  </si>
+  <si>
+    <t>NoOfOccupant</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>IsPolicVerificationDone</t>
+  </si>
+  <si>
+    <t>isDocumentSubmitted</t>
+  </si>
+  <si>
+    <t>MemberId</t>
+  </si>
+  <si>
+    <t>C402</t>
+  </si>
+  <si>
+    <t>TC402</t>
+  </si>
+  <si>
+    <t>OccupantDetails</t>
+  </si>
+  <si>
+    <t>C502-001</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>C502-002</t>
+  </si>
+  <si>
+    <t>C502-003</t>
+  </si>
+  <si>
+    <t>C502-004</t>
+  </si>
+  <si>
+    <t>C502-005</t>
+  </si>
+  <si>
+    <t>Ami Mehta</t>
+  </si>
+  <si>
+    <t>Nameet Mehta</t>
+  </si>
+  <si>
+    <t>Tarak Mehta</t>
+  </si>
+  <si>
+    <t>Daksha Mehta</t>
+  </si>
+  <si>
+    <t>amidave81@yahoo.com</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Retired</t>
+  </si>
+  <si>
+    <t>isSelfOccupant</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>5, 6</t>
+  </si>
+  <si>
+    <t>TC402-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vijay </t>
+  </si>
+  <si>
+    <t>Chavan</t>
+  </si>
+  <si>
+    <t>Vijay Chavan</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Wife</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>vijaychavan@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +429,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -246,10 +463,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,8 +479,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -590,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:BT18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="BM15" sqref="BM15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,9 +832,38 @@
     <col min="19" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.140625" customWidth="1"/>
+    <col min="28" max="28" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="12.140625" customWidth="1"/>
+    <col min="52" max="52" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -624,8 +873,25 @@
       <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Z1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA1" s="3"/>
+      <c r="AM1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN1" s="3"/>
+      <c r="AO1" s="3"/>
+      <c r="AW1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
+      <c r="BM1" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -680,8 +946,131 @@
       <c r="W2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Z2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BR2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -724,8 +1113,95 @@
       <c r="W3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>2</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG3">
+        <v>9881497442</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN3">
+        <v>2</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ3">
+        <v>502</v>
+      </c>
+      <c r="AR3">
+        <v>5</v>
+      </c>
+      <c r="AS3">
+        <v>1560</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX3">
+        <v>2</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>123</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>124</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BQ3">
+        <v>9881497442</v>
+      </c>
+      <c r="BR3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -768,8 +1244,53 @@
       <c r="W4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AM4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN4">
+        <v>2</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ4">
+        <v>402</v>
+      </c>
+      <c r="AR4">
+        <v>4</v>
+      </c>
+      <c r="AS4">
+        <v>1500</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>121</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>107</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>81</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>111</v>
+      </c>
+      <c r="BQ4">
+        <v>95959879545</v>
+      </c>
+      <c r="BR4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="BS4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -794,21 +1315,97 @@
       <c r="O5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="BM5" t="s">
+        <v>108</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>81</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>112</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>117</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
       <c r="H6">
         <v>3</v>
       </c>
       <c r="I6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="BM6" t="s">
+        <v>109</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>81</v>
+      </c>
+      <c r="BP6" t="s">
+        <v>113</v>
+      </c>
+      <c r="BS6" t="s">
+        <v>118</v>
+      </c>
+      <c r="BT6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
+      <c r="BM7" t="s">
+        <v>110</v>
+      </c>
+      <c r="BN7" t="s">
+        <v>81</v>
+      </c>
+      <c r="BP7" t="s">
+        <v>114</v>
+      </c>
+      <c r="BQ7">
+        <v>7878735252</v>
+      </c>
+      <c r="BS7" t="s">
+        <v>118</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
+      <c r="BM8" t="s">
+        <v>122</v>
+      </c>
+      <c r="BN8" t="s">
+        <v>102</v>
+      </c>
+      <c r="BO8" t="s">
+        <v>103</v>
+      </c>
+      <c r="BP8" t="s">
+        <v>125</v>
+      </c>
+      <c r="BQ8">
+        <v>2929293939</v>
+      </c>
+      <c r="BR8" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="BS8" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -816,7 +1413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -824,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -832,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -857,8 +1454,14 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AF3" r:id="rId1"/>
+    <hyperlink ref="BR3" r:id="rId2"/>
+    <hyperlink ref="BR4" r:id="rId3"/>
+    <hyperlink ref="BR8" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding Bootstrap Framwork for UI
Adding bootstrap framwork which includes:

1) Bootstrap classes added under "resources" folder under "js", "css" &
"fonts" folder.

2) Added new jsp file "NavBar.jsp" which contains the menu bar created
using the bootstrap framework.
</commit_message>
<xml_diff>
--- a/Docs/Technical/DBDesign/Login_Registration.xlsx
+++ b/Docs/Technical/DBDesign/Login_Registration.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
-  <si>
-    <t>User</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="150">
   <si>
     <t>UserId</t>
   </si>
@@ -33,9 +30,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Tenant</t>
-  </si>
-  <si>
     <t>TenantId</t>
   </si>
   <si>
@@ -144,15 +138,9 @@
     <t>manish</t>
   </si>
   <si>
-    <t>Supervisor</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
     <t>Permissions</t>
   </si>
   <si>
@@ -174,9 +162,6 @@
     <t>Site Admin</t>
   </si>
   <si>
-    <t>Members</t>
-  </si>
-  <si>
     <t>Update</t>
   </si>
   <si>
@@ -285,9 +270,6 @@
     <t>FlatTenantId</t>
   </si>
   <si>
-    <t>OwnerDetails</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -412,6 +394,78 @@
   </si>
   <si>
     <t>vijaychavan@yahoo.com</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>CommitteeMember</t>
+  </si>
+  <si>
+    <t>ManagingCommittee</t>
+  </si>
+  <si>
+    <t>Self CRUD and View Only Permissions for Public Links</t>
+  </si>
+  <si>
+    <t>Self &amp; Member CRUD and View only permissions for Public Links and Write access to Committee Level links</t>
+  </si>
+  <si>
+    <t>Self, Member, Committee &amp; Managing Committee and Write access to full site including Managing Committee</t>
+  </si>
+  <si>
+    <t>Self, Member &amp; Committee CRUD and Write access to Full Site excluding managing Committee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full site level Admin access across societies </t>
+  </si>
+  <si>
+    <t>RoleCode</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>User Table</t>
+  </si>
+  <si>
+    <t>Roles Table</t>
+  </si>
+  <si>
+    <t>Tenant / Society Master</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>Special Committee</t>
+  </si>
+  <si>
+    <t>Self &amp; Member CRUD and View only permissions for Public Links and Write access to Special Committee Level links</t>
+  </si>
+  <si>
+    <t>Manish Bhatnagar</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MemberDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -467,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -480,6 +534,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -810,628 +867,768 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BT18"/>
+  <dimension ref="A1:BY18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
-      <selection activeCell="BM15" sqref="BM15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.140625" customWidth="1"/>
-    <col min="28" max="28" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="19" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="12.140625" customWidth="1"/>
-    <col min="52" max="52" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="11" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="11" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.42578125" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="11.140625" customWidth="1"/>
+    <col min="30" max="30" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="19" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="19" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="12.140625" customWidth="1"/>
+    <col min="54" max="54" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="M1" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" s="8"/>
+      <c r="V1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="8"/>
+      <c r="AD1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AR1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="BB1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
+      <c r="BR1" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="X2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA1" s="3"/>
-      <c r="AM1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AW1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="BM1" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="AY2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AZ2" s="2" t="s">
+      <c r="BB2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BK2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="BA2" s="2" t="s">
+      <c r="BL2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="BB2" s="2" t="s">
+      <c r="BM2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="BC2" s="2" t="s">
+      <c r="BN2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BD2" s="2" t="s">
+      <c r="BO2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="BE2" s="2" t="s">
+      <c r="BR2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="BF2" s="2" t="s">
+      <c r="BS2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BV2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BW2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BY2" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1">
+        <v>42736</v>
+      </c>
+      <c r="X3" s="1">
+        <v>43100</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z3">
+        <v>48</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>2</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL3">
+        <v>9881497442</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS3">
+        <v>2</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV3">
+        <v>502</v>
+      </c>
+      <c r="AW3">
+        <v>5</v>
+      </c>
+      <c r="AX3">
+        <v>1560</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>97</v>
+      </c>
+      <c r="BC3">
+        <v>2</v>
+      </c>
+      <c r="BD3" t="s">
         <v>96</v>
       </c>
-      <c r="BG2" s="2" t="s">
+      <c r="BE3" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>118</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>99</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>76</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>7</v>
+      </c>
+      <c r="BV3">
+        <v>9881497442</v>
+      </c>
+      <c r="BW3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>42736</v>
+      </c>
+      <c r="X4" s="1">
+        <v>43465</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z4">
+        <v>125</v>
+      </c>
+      <c r="AA4">
+        <v>2</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS4">
+        <v>2</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV4">
+        <v>402</v>
+      </c>
+      <c r="AW4">
+        <v>4</v>
+      </c>
+      <c r="AX4">
+        <v>1500</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>115</v>
+      </c>
+      <c r="BR4" t="s">
+        <v>101</v>
+      </c>
+      <c r="BS4" t="s">
+        <v>76</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>105</v>
+      </c>
+      <c r="BV4">
+        <v>95959879545</v>
+      </c>
+      <c r="BW4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="BX4" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" t="s">
+        <v>11</v>
+      </c>
+      <c r="S5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>102</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BU5" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX5" t="s">
+        <v>111</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="5">
+        <v>4</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6" t="s">
+        <v>55</v>
+      </c>
+      <c r="BR6" t="s">
+        <v>103</v>
+      </c>
+      <c r="BS6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BU6" t="s">
+        <v>107</v>
+      </c>
+      <c r="BX6" t="s">
+        <v>112</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:77" ht="45" x14ac:dyDescent="0.25">
+      <c r="G7" s="5">
+        <v>5</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" t="s">
+        <v>146</v>
+      </c>
+      <c r="P7" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BS7" t="s">
+        <v>76</v>
+      </c>
+      <c r="BU7" t="s">
+        <v>108</v>
+      </c>
+      <c r="BV7">
+        <v>7878735252</v>
+      </c>
+      <c r="BX7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BY7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="G8" s="5">
+        <v>6</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="BR8" t="s">
+        <v>116</v>
+      </c>
+      <c r="BS8" t="s">
+        <v>96</v>
+      </c>
+      <c r="BT8" t="s">
         <v>97</v>
       </c>
-      <c r="BH2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="BI2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="BJ2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BM2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="BN2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BO2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BP2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="BQ2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="BR2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="BS2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BT2" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3">
+      <c r="BU8" t="s">
+        <v>119</v>
+      </c>
+      <c r="BV8">
+        <v>2929293939</v>
+      </c>
+      <c r="BW8" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="BX8" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>56</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3" s="1">
-        <v>42736</v>
-      </c>
-      <c r="T3" s="1">
-        <v>43100</v>
-      </c>
-      <c r="U3" t="s">
-        <v>21</v>
-      </c>
-      <c r="V3">
-        <v>48</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-      <c r="Z3">
-        <v>1</v>
-      </c>
-      <c r="AA3">
-        <v>2</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF3" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG3">
-        <v>9881497442</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN3">
-        <v>2</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ3">
-        <v>502</v>
-      </c>
-      <c r="AR3">
-        <v>5</v>
-      </c>
-      <c r="AS3">
-        <v>1560</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AX3">
-        <v>2</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>123</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>124</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>81</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>9</v>
-      </c>
-      <c r="BQ3">
-        <v>9881497442</v>
-      </c>
-      <c r="BR3" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>116</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4">
-        <v>2</v>
-      </c>
-      <c r="S4" s="1">
-        <v>42736</v>
-      </c>
-      <c r="T4" s="1">
-        <v>43465</v>
-      </c>
-      <c r="U4" t="s">
-        <v>27</v>
-      </c>
-      <c r="V4">
-        <v>125</v>
-      </c>
-      <c r="W4">
-        <v>2</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AN4">
-        <v>2</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ4">
-        <v>402</v>
-      </c>
-      <c r="AR4">
+      <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AS4">
-        <v>1500</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>121</v>
-      </c>
-      <c r="BM4" t="s">
-        <v>107</v>
-      </c>
-      <c r="BN4" t="s">
-        <v>81</v>
-      </c>
-      <c r="BP4" t="s">
-        <v>111</v>
-      </c>
-      <c r="BQ4">
-        <v>95959879545</v>
-      </c>
-      <c r="BR4" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="BS4" t="s">
-        <v>116</v>
-      </c>
-      <c r="BT4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM5" t="s">
-        <v>108</v>
-      </c>
-      <c r="BN5" t="s">
-        <v>81</v>
-      </c>
-      <c r="BP5" t="s">
-        <v>112</v>
-      </c>
-      <c r="BS5" t="s">
-        <v>117</v>
-      </c>
-      <c r="BT5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BM6" t="s">
-        <v>109</v>
-      </c>
-      <c r="BN6" t="s">
-        <v>81</v>
-      </c>
-      <c r="BP6" t="s">
-        <v>113</v>
-      </c>
-      <c r="BS6" t="s">
-        <v>118</v>
-      </c>
-      <c r="BT6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="BM7" t="s">
-        <v>110</v>
-      </c>
-      <c r="BN7" t="s">
-        <v>81</v>
-      </c>
-      <c r="BP7" t="s">
-        <v>114</v>
-      </c>
-      <c r="BQ7">
-        <v>7878735252</v>
-      </c>
-      <c r="BS7" t="s">
-        <v>118</v>
-      </c>
-      <c r="BT7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="BM8" t="s">
-        <v>122</v>
-      </c>
-      <c r="BN8" t="s">
-        <v>102</v>
-      </c>
-      <c r="BO8" t="s">
-        <v>103</v>
-      </c>
-      <c r="BP8" t="s">
-        <v>125</v>
-      </c>
-      <c r="BQ8">
-        <v>2929293939</v>
-      </c>
-      <c r="BR8" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="BS8" t="s">
-        <v>116</v>
-      </c>
-      <c r="BT8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1439,7 +1636,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1447,18 +1644,22 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="V1:W1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AF3" r:id="rId1"/>
-    <hyperlink ref="BR3" r:id="rId2"/>
-    <hyperlink ref="BR4" r:id="rId3"/>
-    <hyperlink ref="BR8" r:id="rId4"/>
+    <hyperlink ref="AK3" r:id="rId1"/>
+    <hyperlink ref="BW3" r:id="rId2"/>
+    <hyperlink ref="BW4" r:id="rId3"/>
+    <hyperlink ref="BW8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1469,16 +1670,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="101" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -1486,42 +1687,42 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1535,16 +1736,18 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1557,16 +1760,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5">
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1578,17 +1783,19 @@
       <c r="F5" s="5">
         <v>3</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="5"/>
+      <c r="G5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5">
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1600,19 +1807,21 @@
         <v>4</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="5"/>
+        <v>127</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5">
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="M6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1620,19 +1829,25 @@
       <c r="B7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="F7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5">
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="M7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Society Registration Workflow
Added Society Registration form but there are some issues to be fixed.
</commit_message>
<xml_diff>
--- a/Docs/Technical/DBDesign/Login_Registration.xlsx
+++ b/Docs/Technical/DBDesign/Login_Registration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="165">
   <si>
     <t>UserId</t>
   </si>
@@ -33,9 +33,6 @@
     <t>TenantId</t>
   </si>
   <si>
-    <t>MTM Infotech</t>
-  </si>
-  <si>
     <t>ContactPerson</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>mmehta</t>
   </si>
   <si>
-    <t>CEO</t>
-  </si>
-  <si>
     <t>Mtm</t>
   </si>
   <si>
@@ -456,16 +450,67 @@
     <t>Self &amp; Member CRUD and View only permissions for Public Links and Write access to Special Committee Level links</t>
   </si>
   <si>
-    <t>Manish Bhatnagar</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
     <t>MemberDetails</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>vatika</t>
+  </si>
+  <si>
+    <t>BuildingCode</t>
+  </si>
+  <si>
+    <t>BuildingName</t>
+  </si>
+  <si>
+    <t>DisplayLabel</t>
+  </si>
+  <si>
+    <t>Amboli</t>
+  </si>
+  <si>
+    <t>StartingFlatNo</t>
+  </si>
+  <si>
+    <t>EndingFlatNo</t>
+  </si>
+  <si>
+    <t>No of Floors</t>
+  </si>
+  <si>
+    <t>FlatsPerFloor</t>
+  </si>
+  <si>
+    <t>RefugueFloor(s)</t>
+  </si>
+  <si>
+    <t>FlatsInRefugueArea</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Champa</t>
+  </si>
+  <si>
+    <t>Chameli</t>
+  </si>
+  <si>
+    <t>Total Flats</t>
+  </si>
+  <si>
+    <t>BuildingMaster</t>
+  </si>
+  <si>
+    <t>onkar</t>
+  </si>
+  <si>
+    <t>bhatnagar</t>
   </si>
 </sst>
 </file>
@@ -867,104 +912,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BY18"/>
+  <dimension ref="A1:BZ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="51.7109375" customWidth="1"/>
     <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.42578125" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="11.140625" customWidth="1"/>
-    <col min="30" max="30" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="19" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="19" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="53" width="12.140625" customWidth="1"/>
-    <col min="54" max="54" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="11" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="12" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="11.140625" customWidth="1"/>
+    <col min="31" max="31" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="19" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="19" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H1" s="6"/>
-      <c r="M1" s="8" t="s">
-        <v>142</v>
-      </c>
       <c r="N1" s="8"/>
-      <c r="V1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="W1" s="8"/>
-      <c r="AD1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="AE1" s="3"/>
+      <c r="O1" s="8"/>
+      <c r="W1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="8"/>
+      <c r="AE1" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="AF1" s="3"/>
-      <c r="AR1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AS1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AS1" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="AT1" s="3"/>
-      <c r="BB1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BC1" s="3"/>
+      <c r="AU1" s="3"/>
+      <c r="BC1" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="BD1" s="3"/>
-      <c r="BR1" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="BE1" s="3"/>
+      <c r="BS1" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -975,634 +1022,796 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>134</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="W2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="BV2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BY2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T3" t="s">
+        <v>49</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1">
+        <v>42736</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>43100</v>
+      </c>
+      <c r="Z3" t="s">
         <v>18</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AA3">
+        <v>48</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>2</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM3">
+        <v>9881497442</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT3">
+        <v>2</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW3">
+        <v>502</v>
+      </c>
+      <c r="AX3">
+        <v>5</v>
+      </c>
+      <c r="AY3">
+        <v>1560</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD3">
+        <v>2</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>94</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>115</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>116</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>97</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>74</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>6</v>
+      </c>
+      <c r="BW3">
+        <v>9881497442</v>
+      </c>
+      <c r="BX3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>108</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:78" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="AG2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BC2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="BD2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="BE2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BF2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="BG2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BI2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="BJ2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="BK2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="BL2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="BN2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BO2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BR2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BS2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="BT2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="BU2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="BV2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BW2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="BX2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="BY2" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S3" t="s">
-        <v>51</v>
-      </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1">
-        <v>42736</v>
-      </c>
-      <c r="X3" s="1">
-        <v>43100</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z3">
-        <v>48</v>
-      </c>
-      <c r="AA3">
-        <v>1</v>
-      </c>
-      <c r="AD3">
-        <v>1</v>
-      </c>
-      <c r="AE3">
-        <v>2</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL3">
-        <v>9881497442</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AS3">
-        <v>2</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AV3">
-        <v>502</v>
-      </c>
-      <c r="AW3">
-        <v>5</v>
-      </c>
-      <c r="AX3">
-        <v>1560</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>81</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BC3">
-        <v>2</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>96</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>117</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>118</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>99</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>76</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>7</v>
-      </c>
-      <c r="BV3">
-        <v>9881497442</v>
-      </c>
-      <c r="BW3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>110</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:77" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" s="5">
-        <v>2</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>136</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
       <c r="N4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" t="s">
         <v>9</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>10</v>
       </c>
-      <c r="P4" t="s">
-        <v>11</v>
-      </c>
-      <c r="S4" t="s">
-        <v>51</v>
-      </c>
-      <c r="V4">
+      <c r="T4" t="s">
+        <v>49</v>
+      </c>
+      <c r="W4">
         <v>2</v>
       </c>
-      <c r="W4" s="1">
+      <c r="X4" s="1">
         <v>42736</v>
       </c>
-      <c r="X4" s="1">
+      <c r="Y4" s="1">
         <v>43465</v>
       </c>
-      <c r="Y4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z4">
+      <c r="Z4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA4">
         <v>125</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>2</v>
       </c>
-      <c r="AR4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AS4">
+      <c r="AS4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT4">
         <v>2</v>
       </c>
-      <c r="AT4" t="s">
-        <v>114</v>
-      </c>
       <c r="AU4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AV4">
+        <v>112</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW4">
         <v>402</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <v>4</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <v>1500</v>
       </c>
-      <c r="AY4" t="s">
-        <v>115</v>
-      </c>
-      <c r="BR4" t="s">
-        <v>101</v>
+      <c r="AZ4" t="s">
+        <v>113</v>
       </c>
       <c r="BS4" t="s">
-        <v>76</v>
-      </c>
-      <c r="BU4" t="s">
-        <v>105</v>
-      </c>
-      <c r="BV4">
+        <v>99</v>
+      </c>
+      <c r="BT4" t="s">
+        <v>74</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BW4">
         <v>95959879545</v>
       </c>
-      <c r="BW4" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>110</v>
+      <c r="BX4" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="BY4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="BZ4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:78" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>136</v>
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
-      </c>
-      <c r="G5" s="5">
-        <v>3</v>
+        <v>133</v>
+      </c>
+      <c r="F5" t="s">
+        <v>145</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M5">
         <v>2</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="O5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="P5" t="s">
         <v>11</v>
       </c>
-      <c r="S5" t="s">
-        <v>51</v>
-      </c>
-      <c r="BR5" t="s">
-        <v>102</v>
+      <c r="Q5" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" t="s">
+        <v>49</v>
       </c>
       <c r="BS5" t="s">
-        <v>76</v>
-      </c>
-      <c r="BU5" t="s">
-        <v>106</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>111</v>
+        <v>100</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BV5" t="s">
+        <v>104</v>
       </c>
       <c r="BY5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:78" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
       <c r="E6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G6" s="5">
-        <v>4</v>
+        <v>134</v>
+      </c>
+      <c r="F6" t="s">
+        <v>145</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M6">
         <v>3</v>
       </c>
       <c r="N6" t="s">
+        <v>164</v>
+      </c>
+      <c r="O6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BS6" t="s">
+        <v>101</v>
+      </c>
+      <c r="BT6" t="s">
+        <v>74</v>
+      </c>
+      <c r="BV6" t="s">
+        <v>105</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>110</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:78" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AS7" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="BS7" t="s">
+        <v>102</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>74</v>
+      </c>
+      <c r="BV7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BW7">
+        <v>7878735252</v>
+      </c>
+      <c r="BY7" t="s">
+        <v>110</v>
+      </c>
+      <c r="BZ7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="H8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BR6" t="s">
-        <v>103</v>
-      </c>
-      <c r="BS6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BU6" t="s">
-        <v>107</v>
-      </c>
-      <c r="BX6" t="s">
-        <v>112</v>
-      </c>
-      <c r="BY6" t="s">
+      <c r="AT8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AW8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AX8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AZ8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="BA8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="BB8" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BC8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="BD8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="BS8" t="s">
+        <v>114</v>
+      </c>
+      <c r="BT8" t="s">
+        <v>94</v>
+      </c>
+      <c r="BU8" t="s">
+        <v>95</v>
+      </c>
+      <c r="BV8" t="s">
+        <v>117</v>
+      </c>
+      <c r="BW8">
+        <v>2929293939</v>
+      </c>
+      <c r="BX8" s="7" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="7" spans="1:77" ht="45" x14ac:dyDescent="0.25">
-      <c r="G7" s="5">
-        <v>5</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" t="s">
-        <v>146</v>
-      </c>
-      <c r="P7" t="s">
-        <v>147</v>
-      </c>
-      <c r="BR7" t="s">
-        <v>104</v>
-      </c>
-      <c r="BS7" t="s">
-        <v>76</v>
-      </c>
-      <c r="BU7" t="s">
+      <c r="BY8" t="s">
         <v>108</v>
       </c>
-      <c r="BV7">
-        <v>7878735252</v>
-      </c>
-      <c r="BX7" t="s">
-        <v>112</v>
-      </c>
-      <c r="BY7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="G8" s="5">
-        <v>6</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="BR8" t="s">
-        <v>116</v>
-      </c>
-      <c r="BS8" t="s">
-        <v>96</v>
-      </c>
-      <c r="BT8" t="s">
-        <v>97</v>
-      </c>
-      <c r="BU8" t="s">
-        <v>119</v>
-      </c>
-      <c r="BV8">
-        <v>2929293939</v>
-      </c>
-      <c r="BW8" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="BX8" t="s">
-        <v>110</v>
-      </c>
-      <c r="BY8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="BZ8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="AS9">
+        <v>1</v>
+      </c>
+      <c r="AT9">
+        <v>2</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX9">
+        <v>101</v>
+      </c>
+      <c r="AY9">
+        <v>1104</v>
+      </c>
+      <c r="AZ9">
+        <v>11</v>
+      </c>
+      <c r="BA9">
+        <v>4</v>
+      </c>
+      <c r="BB9">
+        <v>7</v>
+      </c>
+      <c r="BC9">
+        <v>2</v>
+      </c>
+      <c r="BD9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="AS10">
+        <v>2</v>
+      </c>
+      <c r="AT10">
+        <v>2</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>157</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>159</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX10">
+        <v>101</v>
+      </c>
+      <c r="AY10">
+        <v>1104</v>
+      </c>
+      <c r="AZ10">
+        <v>11</v>
+      </c>
+      <c r="BA10">
+        <v>4</v>
+      </c>
+      <c r="BB10">
+        <v>7</v>
+      </c>
+      <c r="BC10">
+        <v>2</v>
+      </c>
+      <c r="BD10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="AS11">
+        <v>3</v>
+      </c>
+      <c r="AT11">
+        <v>2</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>158</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX11">
+        <v>101</v>
+      </c>
+      <c r="AY11">
+        <v>1104</v>
+      </c>
+      <c r="AZ11">
+        <v>11</v>
+      </c>
+      <c r="BA11">
+        <v>4</v>
+      </c>
+      <c r="BB11">
+        <v>7</v>
+      </c>
+      <c r="BC11">
+        <v>2</v>
+      </c>
+      <c r="BD11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1610,25 +1819,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1636,7 +1845,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1644,7 +1853,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1652,14 +1861,14 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="W1:X1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AK3" r:id="rId1"/>
-    <hyperlink ref="BW3" r:id="rId2"/>
-    <hyperlink ref="BW4" r:id="rId3"/>
-    <hyperlink ref="BW8" r:id="rId4"/>
+    <hyperlink ref="AL3" r:id="rId1"/>
+    <hyperlink ref="BX3" r:id="rId2"/>
+    <hyperlink ref="BX4" r:id="rId3"/>
+    <hyperlink ref="BX8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1687,42 +1896,42 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
         <v>42</v>
-      </c>
-      <c r="L2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1736,10 +1945,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1747,7 +1956,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1760,10 +1969,10 @@
         <v>2</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1771,7 +1980,7 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1784,10 +1993,10 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -1795,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1807,10 +2016,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1818,10 +2027,10 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" t="s">
         <v>49</v>
-      </c>
-      <c r="M6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1833,10 +2042,10 @@
         <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -1844,10 +2053,10 @@
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>